<commit_message>
#47 #48 테이블 업데이트 : UnitUpgradeAbility, UnitUpdradeCost
- UnitUpgrade -> UnitUpgradeAbility
- UnitUpdradeCost 추가 : 딕셔너리 형태에 편입 불가능
</commit_message>
<xml_diff>
--- a/table/Unit.xlsx
+++ b/table/Unit.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\GameProjects\KGCrash\crash\table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Crash\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30720A95-78E9-4E99-AF26-2110393129A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC64FCF-1269-43A2-9270-4060E6BDE724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="1110" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{BB2F5856-9C3A-4FD9-9335-F401F0663D4E}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{BB2F5856-9C3A-4FD9-9335-F401F0663D4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit" sheetId="4" r:id="rId1"/>
-    <sheet name="UnitUpgrade" sheetId="5" r:id="rId2"/>
+    <sheet name="UnitUpgradeAbility" sheetId="5" r:id="rId2"/>
     <sheet name="Skill" sheetId="6" r:id="rId3"/>
     <sheet name="Projectile" sheetId="7" r:id="rId4"/>
+    <sheet name="UnitUpgradeCost" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -231,6 +232,34 @@
   </si>
   <si>
     <t>Targeting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPGRADE_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPGRADE_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPGRADE_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPGRADE_7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPGRADE_8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPGRADE_9</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -238,7 +267,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +285,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
@@ -286,7 +323,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -295,6 +332,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,7 +874,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1049,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3499CA7-C0C0-49AE-B576-80FEEDB8A9A2}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1104,4 +1144,128 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220ED6E0-30BD-4D56-950C-986B1C9E2B09}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13">
+        <v>3000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#91 유닛 테이블 AttackType Enum 필드 추가
</commit_message>
<xml_diff>
--- a/table/Unit.xlsx
+++ b/table/Unit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\GameProjects\KGCrash\crash\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E843F4C7-BE76-4455-9A8E-C1AAC2BBA8B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6323C5-0255-48D7-BE15-0E723B4DF650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6615" yWindow="2835" windowWidth="21600" windowHeight="11385" xr2:uid="{BB2F5856-9C3A-4FD9-9335-F401F0663D4E}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -308,6 +308,21 @@
   </si>
   <si>
     <t>client</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>client</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Projectile</t>
+  </si>
+  <si>
+    <t>Projectile</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -703,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E79B08-4E2A-4909-AFD0-8A046CEA2CED}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -718,7 +733,7 @@
     <col min="11" max="11" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -767,8 +782,11 @@
       <c r="P1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -817,8 +835,11 @@
       <c r="P2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -867,8 +888,11 @@
       <c r="P3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -917,8 +941,11 @@
       <c r="P4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -967,8 +994,11 @@
       <c r="P5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1017,8 +1047,11 @@
       <c r="P6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1066,6 +1099,9 @@
       </c>
       <c r="P7">
         <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>